<commit_message>
Co-authored-by: DE BRAY Pauline <pauline.de_bray@ensam.eu> Co-authored-by: DE WINNE Jef <jef.de_winne@ensam.eu> Co-authored-by: DE BRAY Claire <claire.de_bray@ensam.eu>
</commit_message>
<xml_diff>
--- a/OF.xlsx
+++ b/OF.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7200" yWindow="885" windowWidth="21600" windowHeight="11325" tabRatio="600" firstSheet="3" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="verrin" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,17 +11,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bouteille" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Structure " sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bouchon" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table " sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="casserole" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tablette" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tortue" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ecran" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clavier" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grskjbvj" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tour" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="zlfken" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="zfkn" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="casserole" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tablette" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ecran" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clavier" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chaise" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Radiateur" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -444,14 +439,14 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="22.453125" customWidth="1" min="1" max="1"/>
-    <col width="15.08984375" customWidth="1" min="2" max="2"/>
+    <col width="22.42578125" customWidth="1" min="1" max="1"/>
+    <col width="15.140625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -517,13 +512,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>10h06</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -537,13 +530,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>10h07</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>342</v>
       </c>
     </row>
     <row r="7">
@@ -557,13 +548,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>10h08</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -577,13 +566,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10h09</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -597,13 +584,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>10h10</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -617,13 +602,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">tour </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>10h11</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="11">
@@ -637,13 +620,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>10h12</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="12">
@@ -657,13 +638,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>10h13</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -677,13 +656,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>10h14</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>897</v>
       </c>
     </row>
     <row r="14">
@@ -697,13 +674,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10h15</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -717,13 +692,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>10h16</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>867</v>
       </c>
     </row>
     <row r="16">
@@ -737,13 +710,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>10h17</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="17">
@@ -757,13 +728,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>10h18</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -777,13 +746,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>10h19</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="19">
@@ -797,13 +764,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>10h20</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -817,13 +782,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>10h21</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -841,10 +804,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -853,7 +816,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>314</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2">
@@ -863,7 +826,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4135</v>
+        <v>25245</v>
       </c>
     </row>
     <row r="3">
@@ -873,7 +836,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>365</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -906,17 +869,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ebavurage</t>
+          <t>fraisage</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>assemblage</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -934,10 +897,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -946,7 +909,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1343</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -956,7 +919,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3424</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3">
@@ -966,7 +929,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4">
@@ -999,592 +962,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ebavurage 1</t>
+          <t>ED</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Assemblage</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coût (€)</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Resistance (MPa)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temps de cycle moyen (min) </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gamme fabrication</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nom operation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Temps fabrication</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>3 axes</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Assemble</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>mains</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coût (€)</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Resistance (MPa)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temps de cycle moyen (min) </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gamme fabrication</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nom operation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Temps fabrication</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>rzlkgnz</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jodzbv</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coût (€)</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Resistance (MPa)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temps de cycle moyen (min) </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gamme fabrication</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nom operation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Temps fabrication</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>zkjfzb</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>da</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>erg</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ger</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>erge</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>reg</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coût (€)</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Resistance (MPa)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temps de cycle moyen (min) </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gamme fabrication</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nom operation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Temps fabrication</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>zrlkng</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Metrologie</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>khzf</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Forge</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Coût (€)</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Resistance (MPa)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temps de cycle moyen (min) </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Gamme fabrication</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Nom operation</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Temps fabrication</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>vrjvb</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Forge</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ef</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>rzljg</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Usinage</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>zef</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -1601,13 +989,13 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="22.453125" customWidth="1" min="1" max="1"/>
+    <col width="22.42578125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1663,8 +1051,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1673,18 +1063,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12h56</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1693,18 +1085,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13h05</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1713,18 +1107,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13h21</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1733,12 +1129,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13h51</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1753,13 +1149,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>tour</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>13h54</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1776,10 +1170,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1844,13 +1238,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fonderie</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1h34</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -1864,13 +1256,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fraiseuse</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1h45</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -1884,13 +1274,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>assemblage</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1h56</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1907,13 +1295,13 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="22.453125" customWidth="1" min="1" max="1"/>
-    <col width="15.08984375" customWidth="1" min="2" max="2"/>
+    <col width="22.42578125" customWidth="1" min="1" max="1"/>
+    <col width="15.140625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1943,7 +1331,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
@@ -1969,8 +1357,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>1</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1979,18 +1369,18 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>8h00</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>2</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1999,18 +1389,18 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>8h04</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -2019,18 +1409,18 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>8h08</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>4</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2039,18 +1429,18 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>8h40</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2059,18 +1449,18 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">fraiseuse </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>8h45</t>
-        </is>
+          <t>Emboutisseuse</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>6</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2079,18 +1469,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>tour</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>9h06</t>
-        </is>
+          <t>Emboutisseuse</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>7</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -2099,18 +1489,18 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">tour </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>9h08</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>8</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -2119,18 +1509,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>9h12</t>
-        </is>
+          <t>Emboutisseuse</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>9</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -2139,18 +1529,18 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>9h17</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>10</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2159,33 +1549,31 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>9h20</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>11</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>assemblage 4</t>
+          <t>rabotage1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">assemblage </t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>9h30</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2203,10 +1591,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2273,13 +1661,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fonderie</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>4h34</t>
-        </is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2293,13 +1679,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2318,7 +1704,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3145</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="3">
@@ -2361,39 +1747,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>coulée1</t>
+          <t>coulée 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
+          <t>Emboutisseuse</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>assemblage</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>assemblage</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>5</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -2408,13 +1772,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2423,7 +1787,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>345</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="2">
@@ -2433,7 +1797,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4535</v>
+        <v>5422</v>
       </c>
     </row>
     <row r="3">
@@ -2443,28 +1807,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>N° OF</t>
+          <t>Gamme fabrication</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nom_OF</t>
+          <t>Nom operation</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Machine_OF</t>
+          <t>Machine</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Debut OF</t>
+          <t>Temps fabrication</t>
         </is>
       </c>
     </row>
@@ -2476,18 +1840,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>coulée 1</t>
+          <t>ebavurage 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">fonderie </t>
+          <t>Degauchisseuse</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>45</t>
-        </is>
+          <t>23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>assemblage1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Four</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2501,13 +1883,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2516,7 +1898,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4554</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2">
@@ -2526,7 +1908,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5422</v>
+        <v>4135</v>
       </c>
     </row>
     <row r="3">
@@ -2536,7 +1918,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4">
@@ -2562,39 +1944,25 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ebavurage 1</t>
+          <t>Ebavurage</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fonderie</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>assemblage1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>assemblage</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>34</v>
+          <t>Degauchisseuse</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2611,10 +1979,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2623,7 +1991,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>245</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="2">
@@ -2633,7 +2001,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="3">
@@ -2643,7 +2011,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>245</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -2676,17 +2044,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ebavurage</t>
+          <t>Ebavurage 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>assemblage</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Co-authored-by: DE BRAY Pauline <pauline.de_bray@ensam.eu>
</commit_message>
<xml_diff>
--- a/OF.xlsx
+++ b/OF.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="verrin" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chappe" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chape" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bouteille" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Structure " sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bouchon" sheetId="5" state="visible" r:id="rId5"/>
@@ -17,6 +17,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clavier" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chaise" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Radiateur" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Support de skate" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -981,6 +982,143 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Coût (€)</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Resistance (MPa)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Temps de cycle moyen (min) </t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gamme fabrication</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nom operation</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Machine</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Temps fabrication</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Moulage</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Moulage automatique</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Usinage</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Fraiseuse 3 axes manuelle</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Finition</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Fraiseuse 3 axes manuelle</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1063,7 +1201,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Four</t>
+          <t>Fraiseuse 3 axes manuelle</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1085,7 +1223,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Four</t>
+          <t>Fraiseuse 3 axes manuelle</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1107,7 +1245,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Four</t>
+          <t>Fraiseuse 3 axes manuelle</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1129,7 +1267,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Four</t>
+          <t>Fraiseuse 3 axes manuelle</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1139,8 +1277,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>5</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1149,11 +1289,13 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Four</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>8</v>
+          <t>Fraiseuse 3 axes manuelle</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour finale 2022-2023
Ceci est (normalement) la dernière mise à jour de l'année scolaire 2022-2023
Des bugs mineurs ainsi que l'ajout du Jumeau numérique d'assemblage ont été retouchés.
</commit_message>
<xml_diff>
--- a/OF.xlsx
+++ b/OF.xlsx
@@ -1798,16 +1798,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>coulée</t>
+          <t>Emboutissage</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Four</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
+          <t>Emboutisseuse</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>